<commit_message>
Update test files for workshop script
</commit_message>
<xml_diff>
--- a/DataValueClustering/workshop/workshop_files/analysis_forms/Fragebogen zum Clustering.xlsx
+++ b/DataValueClustering/workshop/workshop_files/analysis_forms/Fragebogen zum Clustering.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>FragebogenZumClustering_Id</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Hans Hansen</t>
-  </si>
-  <si>
-    <t>PartnerAlias</t>
   </si>
 </sst>
 </file>
@@ -410,15 +407,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,110 +423,95 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="I2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
+      <c r="C2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="I3" s="4"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="I4" s="4"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="I5" s="4"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
+      <c r="C5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>